<commit_message>
Added tournament xlsx files and the neptune id to agents csv file
</commit_message>
<xml_diff>
--- a/testtourn2.xlsx
+++ b/testtourn2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ConnectFourRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E08FEA-043C-44F6-A06A-7639CA4A0C4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5341B6A9-24A4-4DAC-94CA-AA3B4A00B838}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="20">
   <si>
     <t>Model</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>AVRWINRATE</t>
+  </si>
+  <si>
+    <t>OpponentWin</t>
   </si>
 </sst>
 </file>
@@ -176,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -184,14 +187,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -234,18 +237,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9CE80C0-4CA9-4CF2-B4CA-9336768BA3F9}" name="Tabel1" displayName="Tabel1" ref="A1:E45" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E45" xr:uid="{68F0084A-8718-47E2-8B05-3A7286DCB820}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9CE80C0-4CA9-4CF2-B4CA-9336768BA3F9}" name="Tabel1" displayName="Tabel1" ref="A1:F45" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:F45" xr:uid="{68F0084A-8718-47E2-8B05-3A7286DCB820}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E45">
     <sortCondition ref="A1:A45"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3ECA7FA0-C57F-4BAF-991F-4D72AB403F75}" name="Model"/>
     <tableColumn id="2" xr3:uid="{86BEEECB-3E83-49FB-937A-AD6918B8C17D}" name="Opponent"/>
     <tableColumn id="3" xr3:uid="{EA471408-CA81-4F7F-A227-F1770114EAB4}" name="Win rate"/>
     <tableColumn id="4" xr3:uid="{16AF891F-4F95-437F-A980-2ED95855E7FF}" name="Tie rate"/>
     <tableColumn id="5" xr3:uid="{E8D10835-B069-448F-8823-73E9B3A45881}" name="ModelWin">
       <calculatedColumnFormula>IF(C2&gt;0.5, 1,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{42040EC2-2CDE-4135-AC8F-041D2BB26A4B}" name="OpponentWin" dataDxfId="0">
+      <calculatedColumnFormula>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -540,7 +546,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L26:L27"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +579,9 @@
       <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="I1" t="s">
         <v>0</v>
       </c>
@@ -610,8 +618,12 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E45" si="0">IF(C2&gt;0.5, 1,0)</f>
-        <v>1</v>
+        <f>IF(C2&gt;0.5, 1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
       </c>
       <c r="G2">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
@@ -621,7 +633,7 @@
         <v>4</v>
       </c>
       <c r="J2">
-        <f ca="1">SUMIF(Tabel1[[Model]:[Opponent]],I2,Tabel1[ModelWin])</f>
+        <f>SUMIF(Tabel1[Model],I2,Tabel1[ModelWin])+SUMIF(Tabel1[Opponent],I2,Tabel1[OpponentWin])</f>
         <v>5</v>
       </c>
       <c r="K2" cm="1">
@@ -659,8 +671,12 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="E2:E45" si="0">IF(C3&gt;0.5, 1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
       </c>
       <c r="G3">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
@@ -670,8 +686,8 @@
         <v>10</v>
       </c>
       <c r="J3">
-        <f ca="1">SUMIF(Tabel1[[Model]:[Opponent]],I3,Tabel1[ModelWin])</f>
-        <v>2</v>
+        <f>SUMIF(Tabel1[Model],I3,Tabel1[ModelWin])+SUMIF(Tabel1[Opponent],I3,Tabel1[OpponentWin])</f>
+        <v>6</v>
       </c>
       <c r="K3" cm="1">
         <f t="array" ref="K3">INDEX(Tabel1[Win rate],MATCH(I3,IF(Tabel1[Opponent]=$K$1,Tabel1[Model]),0))</f>
@@ -711,6 +727,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F4">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G4">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.56000000000000005</v>
@@ -719,8 +739,8 @@
         <v>11</v>
       </c>
       <c r="J4">
-        <f ca="1">SUMIF(Tabel1[[Model]:[Opponent]],I4,Tabel1[ModelWin])</f>
-        <v>2</v>
+        <f>SUMIF(Tabel1[Model],I4,Tabel1[ModelWin])+SUMIF(Tabel1[Opponent],I4,Tabel1[OpponentWin])</f>
+        <v>3</v>
       </c>
       <c r="K4" cm="1">
         <f t="array" ref="K4">INDEX(Tabel1[Win rate],MATCH(I4,IF(Tabel1[Opponent]=$K$1,Tabel1[Model]),0))</f>
@@ -760,6 +780,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F5">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G5">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.26</v>
@@ -768,8 +792,8 @@
         <v>7</v>
       </c>
       <c r="J5">
-        <f ca="1">SUMIF(Tabel1[[Model]:[Opponent]],I5,Tabel1[ModelWin])</f>
-        <v>5</v>
+        <f>SUMIF(Tabel1[Model],I5,Tabel1[ModelWin])+SUMIF(Tabel1[Opponent],I5,Tabel1[OpponentWin])</f>
+        <v>6</v>
       </c>
       <c r="K5" cm="1">
         <f t="array" ref="K5">INDEX(Tabel1[Win rate],MATCH(I5,IF(Tabel1[Opponent]=$K$1,Tabel1[Model]),0))</f>
@@ -788,7 +812,7 @@
         <v>1.05</v>
       </c>
       <c r="O5">
-        <f t="shared" si="1"/>
+        <f>(M5+N5)/9</f>
         <v>0.52444444444444449</v>
       </c>
     </row>
@@ -809,6 +833,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F6">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G6">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.49</v>
@@ -817,8 +845,8 @@
         <v>8</v>
       </c>
       <c r="J6">
-        <f ca="1">SUMIF(Tabel1[[Model]:[Opponent]],I6,Tabel1[ModelWin])</f>
-        <v>3</v>
+        <f>SUMIF(Tabel1[Model],I6,Tabel1[ModelWin])+SUMIF(Tabel1[Opponent],I6,Tabel1[OpponentWin])</f>
+        <v>4</v>
       </c>
       <c r="K6" cm="1">
         <f t="array" ref="K6">INDEX(Tabel1[Win rate],MATCH(I6,IF(Tabel1[Opponent]=$K$1,Tabel1[Model]),0))</f>
@@ -858,6 +886,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F7">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G7">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.53</v>
@@ -866,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="J7">
-        <f ca="1">SUMIF(Tabel1[[Model]:[Opponent]],I7,Tabel1[ModelWin])</f>
+        <f>SUMIF(Tabel1[Model],I7,Tabel1[ModelWin])+SUMIF(Tabel1[Opponent],I7,Tabel1[OpponentWin])</f>
         <v>3</v>
       </c>
       <c r="K7" cm="1">
@@ -907,6 +939,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F8">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G8">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.5</v>
@@ -915,7 +951,7 @@
         <v>12</v>
       </c>
       <c r="J8">
-        <f ca="1">SUMIF(Tabel1[[Model]:[Opponent]],I8,Tabel1[ModelWin])</f>
+        <f>SUMIF(Tabel1[Model],I8,Tabel1[ModelWin])+SUMIF(Tabel1[Opponent],I8,Tabel1[OpponentWin])</f>
         <v>1</v>
       </c>
       <c r="K8" cm="1">
@@ -956,6 +992,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F9">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G9">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>6.9999999999999951E-2</v>
@@ -964,8 +1004,8 @@
         <v>9</v>
       </c>
       <c r="J9">
-        <f ca="1">SUMIF(Tabel1[[Model]:[Opponent]],I9,Tabel1[ModelWin])</f>
-        <v>3</v>
+        <f>SUMIF(Tabel1[Model],I9,Tabel1[ModelWin])+SUMIF(Tabel1[Opponent],I9,Tabel1[OpponentWin])</f>
+        <v>5</v>
       </c>
       <c r="K9" cm="1">
         <f t="array" ref="K9">INDEX(Tabel1[Win rate],MATCH(I9,IF(Tabel1[Opponent]=$K$1,Tabel1[Model]),0))</f>
@@ -1005,6 +1045,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F10">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G10">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.84</v>
@@ -1027,6 +1071,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F11">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G11">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.26</v>
@@ -1049,6 +1097,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F12">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G12">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.56000000000000005</v>
@@ -1071,6 +1123,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F13">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G13">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.14000000000000001</v>
@@ -1093,6 +1149,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F14">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G14">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.96</v>
@@ -1115,6 +1175,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F15">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G15">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.18000000000000005</v>
@@ -1137,6 +1201,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F16">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G16">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.27</v>
@@ -1159,6 +1227,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F17">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G17">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.97</v>
@@ -1181,6 +1253,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F18">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G18">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.24</v>
@@ -1203,6 +1279,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F19">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G19">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.45999999999999996</v>
@@ -1225,6 +1305,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F20">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G20">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.39</v>
@@ -1247,6 +1331,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F21">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G21">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.5</v>
@@ -1269,6 +1357,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F22">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G22">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.47</v>
@@ -1291,6 +1383,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F23">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G23">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.31999999999999995</v>
@@ -1313,6 +1409,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F24">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G24">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.95</v>
@@ -1335,6 +1435,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F25">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G25">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>9.9999999999999978E-2</v>
@@ -1357,6 +1461,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F26">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G26">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.55000000000000004</v>
@@ -1379,6 +1487,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F27">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G27">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.55000000000000004</v>
@@ -1401,6 +1513,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F28">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G28">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.49</v>
@@ -1423,6 +1539,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F29">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G29">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.27</v>
@@ -1445,6 +1565,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F30">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G30">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.92</v>
@@ -1467,6 +1591,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F31">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G31">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.16000000000000003</v>
@@ -1489,6 +1617,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F32">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G32">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.49</v>
@@ -1511,6 +1643,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F33">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G33">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.54</v>
@@ -1533,6 +1669,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F34">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G34">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.55000000000000004</v>
@@ -1555,6 +1695,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F35">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G35">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.54</v>
@@ -1577,6 +1721,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F36">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G36">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.5</v>
@@ -1599,6 +1747,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F37">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G37">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.24</v>
@@ -1621,6 +1773,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F38">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G38">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.92999999999999994</v>
@@ -1643,6 +1799,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F39">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G39">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.33999999999999997</v>
@@ -1665,6 +1825,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F40">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G40">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.86</v>
@@ -1687,6 +1851,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F41">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G41">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.24</v>
@@ -1709,6 +1877,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F42">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
+      </c>
       <c r="G42">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.53</v>
@@ -1731,6 +1903,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F43">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G43">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.45999999999999996</v>
@@ -1753,6 +1929,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="F44">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="G44">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>
         <v>0.43000000000000005</v>
@@ -1774,6 +1954,10 @@
       <c r="E45">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="F45">
+        <f>IF(Tabel1[[#This Row],[Win rate]]&lt;0.5,1,0)</f>
+        <v>1</v>
       </c>
       <c r="G45">
         <f>1-Tabel1[[#This Row],[Win rate]]</f>

</xml_diff>